<commit_message>
- Added writing of base-year MIP in structural decomposition.
</commit_message>
<xml_diff>
--- a/Output/Tabelas_Main/Análises/Resultados_2018_20_Closed_Guilhoto.xlsx
+++ b/Output/Tabelas_Main/Análises/Resultados_2018_20_Closed_Guilhoto.xlsx
@@ -6455,7 +6455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -6482,14 +6482,35 @@
           <t>Var. Demanda Final</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Índices de Preços da Produção Total 2018</t>
-        </is>
-      </c>
+      <c r="E1" s="1" t="inlineStr"/>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Índices de Preços da Produção Total 2011</t>
+          <t>Produção 2018</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Produção 2011</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Índices de Preços Produção 2018</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Índices de Preços Produção 2011</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Índices de Preços Demanda 2018</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Índices de Preços Demannda 2011</t>
         </is>
       </c>
     </row>
@@ -6509,10 +6530,25 @@
         <v>55080.68457585883</v>
       </c>
       <c r="E2" t="n">
+        <v>110161.3691517177</v>
+      </c>
+      <c r="F2" t="n">
+        <v>374168.4499906288</v>
+      </c>
+      <c r="G2" t="n">
+        <v>289403</v>
+      </c>
+      <c r="H2" t="n">
         <v>157.1126587542919</v>
       </c>
-      <c r="F2" t="n">
+      <c r="I2" t="n">
         <v>113.042020988034</v>
+      </c>
+      <c r="J2" t="n">
+        <v>159.915803929415</v>
+      </c>
+      <c r="K2" t="n">
+        <v>109.2818651975474</v>
       </c>
     </row>
     <row r="3">
@@ -6531,10 +6567,25 @@
         <v>6553.089615312801</v>
       </c>
       <c r="E3" t="n">
+        <v>13106.1792306256</v>
+      </c>
+      <c r="F3" t="n">
+        <v>223998.4448557381</v>
+      </c>
+      <c r="G3" t="n">
+        <v>208664.9999999999</v>
+      </c>
+      <c r="H3" t="n">
         <v>159.174319370667</v>
       </c>
-      <c r="F3" t="n">
+      <c r="I3" t="n">
         <v>126.4649078666763</v>
+      </c>
+      <c r="J3" t="n">
+        <v>157.0813207813158</v>
+      </c>
+      <c r="K3" t="n">
+        <v>127.8633998524115</v>
       </c>
     </row>
     <row r="4">
@@ -6553,10 +6604,25 @@
         <v>-174240.0822096647</v>
       </c>
       <c r="E4" t="n">
+        <v>-348480.1644193294</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1839593.131353628</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2042528</v>
+      </c>
+      <c r="H4" t="n">
         <v>180.5942272439029</v>
       </c>
-      <c r="F4" t="n">
+      <c r="I4" t="n">
         <v>107.4096413855771</v>
+      </c>
+      <c r="J4" t="n">
+        <v>176.3516981768722</v>
+      </c>
+      <c r="K4" t="n">
+        <v>108.2375505161463</v>
       </c>
     </row>
     <row r="5">
@@ -6575,10 +6641,25 @@
         <v>16199.3700070977</v>
       </c>
       <c r="E5" t="n">
+        <v>32398.74001419541</v>
+      </c>
+      <c r="F5" t="n">
+        <v>204276.6561780074</v>
+      </c>
+      <c r="G5" t="n">
+        <v>159615.0000000001</v>
+      </c>
+      <c r="H5" t="n">
         <v>158.1869441403111</v>
       </c>
-      <c r="F5" t="n">
+      <c r="I5" t="n">
         <v>102.9765372928609</v>
+      </c>
+      <c r="J5" t="n">
+        <v>162.0493692876805</v>
+      </c>
+      <c r="K5" t="n">
+        <v>102.8470377460445</v>
       </c>
     </row>
     <row r="6">
@@ -6597,10 +6678,25 @@
         <v>1474.013061567632</v>
       </c>
       <c r="E6" t="n">
+        <v>2948.026123135265</v>
+      </c>
+      <c r="F6" t="n">
+        <v>44304.6084910782</v>
+      </c>
+      <c r="G6" t="n">
+        <v>45042.00000000002</v>
+      </c>
+      <c r="H6" t="n">
         <v>185.5788885180127</v>
       </c>
-      <c r="F6" t="n">
+      <c r="I6" t="n">
         <v>103.9896096976155</v>
+      </c>
+      <c r="J6" t="n">
+        <v>187.215615688833</v>
+      </c>
+      <c r="K6" t="n">
+        <v>102.2483170247471</v>
       </c>
     </row>
     <row r="7">
@@ -6619,10 +6715,25 @@
         <v>-109011.9554843306</v>
       </c>
       <c r="E7" t="n">
+        <v>-218023.9109686612</v>
+      </c>
+      <c r="F7" t="n">
+        <v>372039.126138331</v>
+      </c>
+      <c r="G7" t="n">
+        <v>477384.0000000001</v>
+      </c>
+      <c r="H7" t="n">
         <v>148.3911129806087</v>
       </c>
-      <c r="F7" t="n">
+      <c r="I7" t="n">
         <v>106.391290868567</v>
+      </c>
+      <c r="J7" t="n">
+        <v>148.2771999627352</v>
+      </c>
+      <c r="K7" t="n">
+        <v>106.3592140841332</v>
       </c>
     </row>
     <row r="8">
@@ -6641,10 +6752,25 @@
         <v>-6933.976998697971</v>
       </c>
       <c r="E8" t="n">
+        <v>-13867.95399739594</v>
+      </c>
+      <c r="F8" t="n">
+        <v>665316.403479839</v>
+      </c>
+      <c r="G8" t="n">
+        <v>670505.0000000002</v>
+      </c>
+      <c r="H8" t="n">
         <v>194.7452359844398</v>
       </c>
-      <c r="F8" t="n">
+      <c r="I8" t="n">
         <v>111.0970089708503</v>
+      </c>
+      <c r="J8" t="n">
+        <v>194.4717908276851</v>
+      </c>
+      <c r="K8" t="n">
+        <v>110.7995597204967</v>
       </c>
     </row>
     <row r="9">
@@ -6663,10 +6789,25 @@
         <v>-4483.68740392636</v>
       </c>
       <c r="E9" t="n">
+        <v>-8967.374807852721</v>
+      </c>
+      <c r="F9" t="n">
+        <v>349051.9612631437</v>
+      </c>
+      <c r="G9" t="n">
+        <v>331903.9999999999</v>
+      </c>
+      <c r="H9" t="n">
         <v>173.4715936873136</v>
       </c>
-      <c r="F9" t="n">
+      <c r="I9" t="n">
         <v>108.2361164674123</v>
+      </c>
+      <c r="J9" t="n">
+        <v>170.899038250212</v>
+      </c>
+      <c r="K9" t="n">
+        <v>106.5827637877585</v>
       </c>
     </row>
     <row r="10">
@@ -6685,10 +6826,25 @@
         <v>9763.909126929044</v>
       </c>
       <c r="E10" t="n">
+        <v>19527.81825385809</v>
+      </c>
+      <c r="F10" t="n">
+        <v>158734.062075812</v>
+      </c>
+      <c r="G10" t="n">
+        <v>151976.0000000001</v>
+      </c>
+      <c r="H10" t="n">
         <v>191.9720292009299</v>
       </c>
-      <c r="F10" t="n">
+      <c r="I10" t="n">
         <v>111.1517608043375</v>
+      </c>
+      <c r="J10" t="n">
+        <v>192.1530169087521</v>
+      </c>
+      <c r="K10" t="n">
+        <v>110.8669483622323</v>
       </c>
     </row>
     <row r="11">
@@ -6707,10 +6863,25 @@
         <v>39564.29663126458</v>
       </c>
       <c r="E11" t="n">
+        <v>79128.59326252916</v>
+      </c>
+      <c r="F11" t="n">
+        <v>322475.2187249137</v>
+      </c>
+      <c r="G11" t="n">
+        <v>267219.0000000001</v>
+      </c>
+      <c r="H11" t="n">
         <v>122.8206004684852</v>
       </c>
-      <c r="F11" t="n">
+      <c r="I11" t="n">
         <v>103.927864410839</v>
+      </c>
+      <c r="J11" t="n">
+        <v>122.9128666236359</v>
+      </c>
+      <c r="K11" t="n">
+        <v>103.3037068185208</v>
       </c>
     </row>
     <row r="12">
@@ -6729,10 +6900,25 @@
         <v>-14972.45775071849</v>
       </c>
       <c r="E12" t="n">
+        <v>-29944.91550143699</v>
+      </c>
+      <c r="F12" t="n">
+        <v>364923.7646214692</v>
+      </c>
+      <c r="G12" t="n">
+        <v>384446</v>
+      </c>
+      <c r="H12" t="n">
         <v>177.8478309498996</v>
       </c>
-      <c r="F12" t="n">
+      <c r="I12" t="n">
         <v>103.5339163367547</v>
+      </c>
+      <c r="J12" t="n">
+        <v>179.1513734236229</v>
+      </c>
+      <c r="K12" t="n">
+        <v>105.468975235646</v>
       </c>
     </row>
     <row r="13">
@@ -6751,10 +6937,25 @@
         <v>45711.31481897608</v>
       </c>
       <c r="E13" t="n">
+        <v>91422.62963795215</v>
+      </c>
+      <c r="F13" t="n">
+        <v>357568.7213230211</v>
+      </c>
+      <c r="G13" t="n">
+        <v>307632.9999999999</v>
+      </c>
+      <c r="H13" t="n">
         <v>178.9172155866675</v>
       </c>
-      <c r="F13" t="n">
+      <c r="I13" t="n">
         <v>110.6380004745915</v>
+      </c>
+      <c r="J13" t="n">
+        <v>178.4291594859991</v>
+      </c>
+      <c r="K13" t="n">
+        <v>110.1848430545836</v>
       </c>
     </row>
     <row r="14">
@@ -6773,10 +6974,25 @@
         <v>796.9524898622158</v>
       </c>
       <c r="E14" t="n">
+        <v>1593.904979724432</v>
+      </c>
+      <c r="F14" t="n">
+        <v>222982.8785016106</v>
+      </c>
+      <c r="G14" t="n">
+        <v>226881.0000000001</v>
+      </c>
+      <c r="H14" t="n">
         <v>177.7374131427482</v>
       </c>
-      <c r="F14" t="n">
+      <c r="I14" t="n">
         <v>108.8614736359589</v>
+      </c>
+      <c r="J14" t="n">
+        <v>185.4336723725266</v>
+      </c>
+      <c r="K14" t="n">
+        <v>100.8110472979885</v>
       </c>
     </row>
     <row r="15">
@@ -6795,10 +7011,25 @@
         <v>9106.100586378971</v>
       </c>
       <c r="E15" t="n">
+        <v>18212.20117275794</v>
+      </c>
+      <c r="F15" t="n">
+        <v>202025.2579015939</v>
+      </c>
+      <c r="G15" t="n">
+        <v>183751</v>
+      </c>
+      <c r="H15" t="n">
         <v>174.8741734917556</v>
       </c>
-      <c r="F15" t="n">
+      <c r="I15" t="n">
         <v>108.4413146050906</v>
+      </c>
+      <c r="J15" t="n">
+        <v>183.2933806887661</v>
+      </c>
+      <c r="K15" t="n">
+        <v>104.7251782285569</v>
       </c>
     </row>
     <row r="16">
@@ -6817,10 +7048,25 @@
         <v>21143.85368054967</v>
       </c>
       <c r="E16" t="n">
+        <v>42287.70736109934</v>
+      </c>
+      <c r="F16" t="n">
+        <v>520167.6802317541</v>
+      </c>
+      <c r="G16" t="n">
+        <v>498838.9999999999</v>
+      </c>
+      <c r="H16" t="n">
         <v>165.09368663916</v>
       </c>
-      <c r="F16" t="n">
+      <c r="I16" t="n">
         <v>104.7201602120123</v>
+      </c>
+      <c r="J16" t="n">
+        <v>164.8091240004831</v>
+      </c>
+      <c r="K16" t="n">
+        <v>104.5710454250277</v>
       </c>
     </row>
     <row r="17">
@@ -6839,10 +7085,25 @@
         <v>1450.91334784667</v>
       </c>
       <c r="E17" t="n">
+        <v>2901.826695693339</v>
+      </c>
+      <c r="F17" t="n">
+        <v>219890.1379463859</v>
+      </c>
+      <c r="G17" t="n">
+        <v>218267.0000000001</v>
+      </c>
+      <c r="H17" t="n">
         <v>224.8995814994567</v>
       </c>
-      <c r="F17" t="n">
+      <c r="I17" t="n">
         <v>117.4492708471734</v>
+      </c>
+      <c r="J17" t="n">
+        <v>224.9004641569068</v>
+      </c>
+      <c r="K17" t="n">
+        <v>118.0270214064947</v>
       </c>
     </row>
     <row r="18">
@@ -6861,10 +7122,25 @@
         <v>29511.4381399497</v>
       </c>
       <c r="E18" t="n">
+        <v>59022.8762798994</v>
+      </c>
+      <c r="F18" t="n">
+        <v>261464.5323712984</v>
+      </c>
+      <c r="G18" t="n">
+        <v>225997</v>
+      </c>
+      <c r="H18" t="n">
         <v>193.3681006041872</v>
       </c>
-      <c r="F18" t="n">
+      <c r="I18" t="n">
         <v>106.2642424456962</v>
+      </c>
+      <c r="J18" t="n">
+        <v>191.7552494877763</v>
+      </c>
+      <c r="K18" t="n">
+        <v>107.0975574004714</v>
       </c>
     </row>
     <row r="19">
@@ -6883,10 +7159,25 @@
         <v>-315.068703756301</v>
       </c>
       <c r="E19" t="n">
+        <v>-630.137407512602</v>
+      </c>
+      <c r="F19" t="n">
+        <v>22172.65735413571</v>
+      </c>
+      <c r="G19" t="n">
+        <v>22924</v>
+      </c>
+      <c r="H19" t="n">
         <v>182.0530546036279</v>
       </c>
-      <c r="F19" t="n">
+      <c r="I19" t="n">
         <v>107.7560635142209</v>
+      </c>
+      <c r="J19" t="n">
+        <v>183.6655333504479</v>
+      </c>
+      <c r="K19" t="n">
+        <v>107.0660861518209</v>
       </c>
     </row>
     <row r="20">
@@ -6905,10 +7196,25 @@
         <v>-7282.700268214883</v>
       </c>
       <c r="E20" t="n">
+        <v>-14565.40053642977</v>
+      </c>
+      <c r="F20" t="n">
+        <v>96409.78284649318</v>
+      </c>
+      <c r="G20" t="n">
+        <v>102672</v>
+      </c>
+      <c r="H20" t="n">
         <v>178.3211152687016</v>
       </c>
-      <c r="F20" t="n">
+      <c r="I20" t="n">
         <v>107.6661601994702</v>
+      </c>
+      <c r="J20" t="n">
+        <v>178.4536190485331</v>
+      </c>
+      <c r="K20" t="n">
+        <v>108.2753537134264</v>
       </c>
     </row>
     <row r="21">
@@ -6927,9 +7233,24 @@
         <v>1625.99975897582</v>
       </c>
       <c r="E21" t="n">
+        <v>3251.999517951641</v>
+      </c>
+      <c r="F21" t="n">
+        <v>42483.99975897581</v>
+      </c>
+      <c r="G21" t="n">
+        <v>40857.99999999999</v>
+      </c>
+      <c r="H21" t="n">
         <v>175.2447990358308</v>
       </c>
-      <c r="F21" t="n">
+      <c r="I21" t="n">
+        <v>108.7522639385188</v>
+      </c>
+      <c r="J21" t="n">
+        <v>175.2447990358308</v>
+      </c>
+      <c r="K21" t="n">
         <v>108.7522639385188</v>
       </c>
     </row>
@@ -6948,12 +7269,31 @@
       <c r="D22" t="n">
         <v>-79257.99297873958</v>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E22" t="n">
+        <v>-158515.9859574792</v>
+      </c>
+      <c r="F22" t="n">
+        <v>6864047.475407857</v>
+      </c>
+      <c r="G22" t="n">
+        <v>6856509</v>
+      </c>
+      <c r="H22" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>